<commit_message>
Add `task-13` in `financial-methematics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/operations-research/course-work/Бронников ПМ-1901 - Моделирование оптимизационных задач средствами динамического программирования.xlsx
+++ b/3-course-6-semester/operations-research/course-work/Бронников ПМ-1901 - Моделирование оптимизационных задач средствами динамического программирования.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\operations-research\course-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F61B9CA-A657-4CAE-BA0C-7F8C86260A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F474C9-71F3-46B3-BC26-D3D4FC4DAFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,23 +886,14 @@
   <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -910,12 +901,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -954,12 +939,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -996,6 +975,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1276,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,225 +1291,229 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" ht="21" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" ht="21" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7">
+      <c r="B5" s="58"/>
+      <c r="C5" s="5">
         <v>228</v>
       </c>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>20</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="29">
         <v>220</v>
       </c>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="D9" s="9"/>
+      <c r="J9" s="1">
+        <f>228/20</f>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>12</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="21">
         <v>130</v>
       </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>16</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="21">
         <v>170</v>
       </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="23">
         <v>5</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="24">
         <v>55</v>
       </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="21" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:10" ht="21" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="13">
         <v>10</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <f>B17*B9</f>
         <v>200</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="33">
         <f>B17*C9</f>
         <v>2200</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <f>B18*B10</f>
         <v>12</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="34">
         <f>B18*C10</f>
         <v>130</v>
       </c>
-      <c r="E18" s="11"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="11">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <f>B19*B11</f>
         <v>0</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="34">
         <f>B19*C11</f>
         <v>0</v>
       </c>
-      <c r="E19" s="11"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="14">
         <v>3</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="15">
         <f>B20*B12</f>
         <v>15</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="36">
         <f>B20*C12</f>
         <v>165</v>
       </c>
-      <c r="E20" s="11"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="48">
+      <c r="B21" s="63"/>
+      <c r="C21" s="41">
         <f>SUM(C17:C20)</f>
         <v>227</v>
       </c>
-      <c r="D21" s="44">
+      <c r="D21" s="37">
         <f>SUM(D17:D20)</f>
         <v>2495</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1530,7 +1534,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="L19:M19"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,186 +1547,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" ht="21" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="11"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="30" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="21">
         <v>0</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>12</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>10</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="21">
         <v>9</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>20</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>16</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>19</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="21">
         <v>17</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>30</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>24</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>30</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>26</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="21">
         <v>25</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>40</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>28</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>35</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>32</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="21">
         <v>32</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28">
+      <c r="A11" s="23">
         <v>6</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="23">
         <v>50</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="23">
         <v>32</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="23">
         <v>37</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="23">
         <v>36</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="24">
         <v>38</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,159 +1744,159 @@
       <c r="E14"/>
     </row>
     <row r="15" spans="1:10" ht="21" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="11"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="44">
         <f>A6</f>
         <v>1</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="45">
         <f>A11</f>
         <v>6</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="53">
+      <c r="B18" s="46">
         <f>B11</f>
         <v>50</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:7" ht="21" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="9"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="11"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="55" t="s">
+      <c r="F24" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="47">
+      <c r="B25" s="40">
         <v>1.0000020000000001</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="40">
         <v>3</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="40">
         <v>3</v>
       </c>
-      <c r="E25" s="47">
+      <c r="E25" s="40">
         <v>2</v>
       </c>
-      <c r="F25" s="57" t="s">
+      <c r="F25" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="46">
+      <c r="B26" s="39">
         <f>INDEX($B$6:$B$11,MATCH(ROUND(B25,1),$A$6:$A$11,0))</f>
         <v>0</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="39">
         <f t="shared" ref="C26:E26" si="0">INDEX($B$6:$B$11,MATCH(ROUND(C25,1),$A$6:$A$11,0))</f>
         <v>20</v>
       </c>
-      <c r="D26" s="46">
+      <c r="D26" s="39">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="39">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F26" s="62">
+      <c r="F26" s="55">
         <f>SUM(B26:E26)</f>
         <v>50</v>
       </c>
-      <c r="G26" s="11"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="60">
+      <c r="B27" s="53">
         <f>INDEX(C$6:C$11,MATCH(ROUND(B25,1),$A$6:$A$11,0))</f>
         <v>0</v>
       </c>
-      <c r="C27" s="60">
+      <c r="C27" s="53">
         <f>INDEX(D$6:D$11,MATCH(ROUND(C25,1),$A$6:$A$11,0))</f>
         <v>22</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="53">
         <f>INDEX(E$6:E$11,MATCH(ROUND(D25,1),$A$6:$A$11,0))</f>
         <v>19</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E27" s="53">
         <f>INDEX(F$6:F$11,MATCH(ROUND(E25,1),$A$6:$A$11,0))</f>
         <v>9</v>
       </c>
-      <c r="F27" s="61">
+      <c r="F27" s="54">
         <f>SUM(B27:E27)</f>
         <v>50</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>